<commit_message>
Deploying to main from @ pedalboard/pedalboard-soundcard@3a51d1952a1cfa062257a61bb80e93aedc8dfe00 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Positional/pedalboard-soundcard-bom.xlsx
+++ b/latest/BoM/Positional/pedalboard-soundcard-bom.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="207">
   <si>
     <t>Row</t>
   </si>
@@ -495,9 +495,6 @@
   </si>
   <si>
     <t>HVQFN-32-1EP_5x5mm_P0.5mm_EP3.1x3.1mm_ThermalVias</t>
-  </si>
-  <si>
-    <t>Package_DFN_QFN</t>
   </si>
   <si>
     <t>https://www.ti.com/lit/ds/symlink/pcm5242.pdf</t>
@@ -1174,7 +1171,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1199,13 +1196,13 @@
     </row>
     <row r="2" spans="1:23">
       <c r="C2" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>94</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F2" s="3">
         <v>18</v>
@@ -1213,41 +1210,41 @@
     </row>
     <row r="3" spans="1:23">
       <c r="C3" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>191</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>199</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:23">
       <c r="C4" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>193</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:23">
       <c r="C5" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>195</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1255,13 +1252,13 @@
     </row>
     <row r="6" spans="1:23">
       <c r="C6" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>197</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F6" s="3">
         <v>72</v>
@@ -2355,7 +2352,7 @@
         <v>158</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>159</v>
+        <v>94</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>23</v>
@@ -2367,7 +2364,7 @@
         <v>32</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M23" s="8" t="s">
         <v>34</v>
@@ -2379,10 +2376,10 @@
         <v>97</v>
       </c>
       <c r="P23" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q23" s="7" t="s">
         <v>161</v>
-      </c>
-      <c r="Q23" s="7" t="s">
-        <v>162</v>
       </c>
       <c r="R23" s="7" t="s">
         <v>53</v>
@@ -2397,30 +2394,30 @@
         <v>42</v>
       </c>
       <c r="V23" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="W23" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:23">
       <c r="A24" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>144</v>
       </c>
       <c r="E24" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="F24" s="11" t="s">
         <v>166</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>167</v>
       </c>
       <c r="G24" s="11" t="s">
         <v>134</v>
@@ -2438,7 +2435,7 @@
         <v>32</v>
       </c>
       <c r="L24" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="M24" s="12" t="s">
         <v>34</v>
@@ -2447,13 +2444,13 @@
         <v>49</v>
       </c>
       <c r="O24" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="P24" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="P24" s="11" t="s">
+      <c r="Q24" s="11" t="s">
         <v>170</v>
-      </c>
-      <c r="Q24" s="11" t="s">
-        <v>171</v>
       </c>
       <c r="R24" s="11" t="s">
         <v>39</v>
@@ -2476,28 +2473,28 @@
     </row>
     <row r="25" spans="1:23">
       <c r="A25" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>144</v>
       </c>
       <c r="E25" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="F25" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="G25" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="H25" s="7" t="s">
         <v>176</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>177</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>23</v>
@@ -2509,7 +2506,7 @@
         <v>32</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M25" s="8" t="s">
         <v>34</v>
@@ -2521,10 +2518,10 @@
         <v>97</v>
       </c>
       <c r="P25" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q25" s="7" t="s">
         <v>179</v>
-      </c>
-      <c r="Q25" s="7" t="s">
-        <v>180</v>
       </c>
       <c r="R25" s="7" t="s">
         <v>53</v>
@@ -2539,36 +2536,36 @@
         <v>42</v>
       </c>
       <c r="V25" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="W25" s="7" t="s">
         <v>181</v>
-      </c>
-      <c r="W25" s="7" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="26" spans="1:23">
       <c r="A26" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>144</v>
       </c>
       <c r="E26" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="F26" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="F26" s="11" t="s">
-        <v>185</v>
-      </c>
       <c r="G26" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="H26" s="11" t="s">
         <v>176</v>
-      </c>
-      <c r="H26" s="11" t="s">
-        <v>177</v>
       </c>
       <c r="I26" s="9" t="s">
         <v>23</v>
@@ -2580,7 +2577,7 @@
         <v>32</v>
       </c>
       <c r="L26" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M26" s="12" t="s">
         <v>34</v>
@@ -2592,10 +2589,10 @@
         <v>97</v>
       </c>
       <c r="P26" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q26" s="11" t="s">
         <v>186</v>
-      </c>
-      <c r="Q26" s="11" t="s">
-        <v>187</v>
       </c>
       <c r="R26" s="11" t="s">
         <v>53</v>
@@ -2610,10 +2607,10 @@
         <v>42</v>
       </c>
       <c r="V26" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="W26" s="11" t="s">
         <v>181</v>
-      </c>
-      <c r="W26" s="11" t="s">
-        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -2639,22 +2636,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-soundcard@f177819ae6f0370ab94271f90f51836291559134 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Positional/pedalboard-soundcard-bom.xlsx
+++ b/latest/BoM/Positional/pedalboard-soundcard-bom.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="206">
   <si>
     <t>Row</t>
   </si>
@@ -546,9 +546,6 @@
   </si>
   <si>
     <t>Oscillator_SMD_Abracon_ASDMB-4Pin_2.5x2.0mm</t>
-  </si>
-  <si>
-    <t>Oscillator</t>
   </si>
   <si>
     <t>https://abracon.com/Oscillators/ASCO.pdf</t>
@@ -1171,7 +1168,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1196,13 +1193,13 @@
     </row>
     <row r="2" spans="1:23">
       <c r="C2" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>94</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F2" s="3">
         <v>18</v>
@@ -1210,41 +1207,41 @@
     </row>
     <row r="3" spans="1:23">
       <c r="C3" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>190</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:23">
       <c r="C4" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:23">
       <c r="C5" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>194</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1252,13 +1249,13 @@
     </row>
     <row r="6" spans="1:23">
       <c r="C6" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>196</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F6" s="3">
         <v>72</v>
@@ -2494,7 +2491,7 @@
         <v>175</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>176</v>
+        <v>94</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>23</v>
@@ -2506,7 +2503,7 @@
         <v>32</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M25" s="8" t="s">
         <v>34</v>
@@ -2518,10 +2515,10 @@
         <v>97</v>
       </c>
       <c r="P25" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q25" s="7" t="s">
         <v>178</v>
-      </c>
-      <c r="Q25" s="7" t="s">
-        <v>179</v>
       </c>
       <c r="R25" s="7" t="s">
         <v>53</v>
@@ -2536,15 +2533,15 @@
         <v>42</v>
       </c>
       <c r="V25" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="W25" s="7" t="s">
         <v>180</v>
-      </c>
-      <c r="W25" s="7" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="26" spans="1:23">
       <c r="A26" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>34</v>
@@ -2556,16 +2553,16 @@
         <v>144</v>
       </c>
       <c r="E26" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="F26" s="11" t="s">
         <v>183</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>184</v>
       </c>
       <c r="G26" s="11" t="s">
         <v>175</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>176</v>
+        <v>94</v>
       </c>
       <c r="I26" s="9" t="s">
         <v>23</v>
@@ -2577,7 +2574,7 @@
         <v>32</v>
       </c>
       <c r="L26" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M26" s="12" t="s">
         <v>34</v>
@@ -2589,10 +2586,10 @@
         <v>97</v>
       </c>
       <c r="P26" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q26" s="11" t="s">
         <v>185</v>
-      </c>
-      <c r="Q26" s="11" t="s">
-        <v>186</v>
       </c>
       <c r="R26" s="11" t="s">
         <v>53</v>
@@ -2607,10 +2604,10 @@
         <v>42</v>
       </c>
       <c r="V26" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="W26" s="11" t="s">
         <v>180</v>
-      </c>
-      <c r="W26" s="11" t="s">
-        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -2636,22 +2633,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-soundcard@99363dd4079ad7a35a02145145f80d1bef758339 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Positional/pedalboard-soundcard-bom.xlsx
+++ b/latest/BoM/Positional/pedalboard-soundcard-bom.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="223">
   <si>
     <t>Row</t>
   </si>
@@ -296,12 +296,18 @@
     <t>pedalboard-soundcard</t>
   </si>
   <si>
-    <t>61.6900</t>
+    <t>59.1500</t>
   </si>
   <si>
     <t>19.1000</t>
   </si>
   <si>
+    <t>180.0000</t>
+  </si>
+  <si>
+    <t>bottom</t>
+  </si>
+  <si>
     <t>THT</t>
   </si>
   <si>
@@ -468,9 +474,6 @@
   </si>
   <si>
     <t>47.5800</t>
-  </si>
-  <si>
-    <t>180.0000</t>
   </si>
   <si>
     <t>3.6000</t>
@@ -1216,7 +1219,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1241,13 +1244,13 @@
     </row>
     <row r="2" spans="1:23">
       <c r="C2" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>91</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F2" s="3">
         <v>18</v>
@@ -1255,41 +1258,41 @@
     </row>
     <row r="3" spans="1:23">
       <c r="C3" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:23">
       <c r="C4" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>215</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:23">
       <c r="C5" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1297,13 +1300,13 @@
     </row>
     <row r="6" spans="1:23">
       <c r="C6" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="F6" s="3">
         <v>72</v>
@@ -1788,45 +1791,45 @@
         <v>93</v>
       </c>
       <c r="R14" s="10" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="S14" s="10" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="T14" s="10" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="U14" s="10" t="s">
         <v>42</v>
       </c>
       <c r="V14" s="10" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="W14" s="10" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:23">
       <c r="A15" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>78</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>91</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>91</v>
@@ -1850,13 +1853,13 @@
         <v>50</v>
       </c>
       <c r="O15" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="P15" s="7" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="Q15" s="7" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="R15" s="7" t="s">
         <v>54</v>
@@ -1865,16 +1868,16 @@
         <v>40</v>
       </c>
       <c r="T15" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="U15" s="7" t="s">
         <v>42</v>
       </c>
       <c r="V15" s="7" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="W15" s="7" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:23" ht="30" customHeight="1">
@@ -1882,52 +1885,52 @@
         <v>58</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>26</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="K16" s="8" t="s">
         <v>32</v>
       </c>
       <c r="L16" s="10" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="M16" s="9" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="N16" s="10" t="s">
         <v>60</v>
       </c>
       <c r="O16" s="8" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="P16" s="10" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="Q16" s="10" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="R16" s="10" t="s">
         <v>54</v>
@@ -1953,25 +1956,25 @@
         <v>48</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>31</v>
@@ -1983,10 +1986,10 @@
         <v>32</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="N17" s="7" t="s">
         <v>35</v>
@@ -1995,10 +1998,10 @@
         <v>36</v>
       </c>
       <c r="P17" s="7" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="Q17" s="7" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="R17" s="7" t="s">
         <v>39</v>
@@ -2021,28 +2024,28 @@
     </row>
     <row r="18" spans="1:23" ht="30" customHeight="1">
       <c r="A18" s="8" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>26</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="I18" s="8" t="s">
         <v>31</v>
@@ -2054,10 +2057,10 @@
         <v>32</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="M18" s="9" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="N18" s="10" t="s">
         <v>50</v>
@@ -2066,10 +2069,10 @@
         <v>36</v>
       </c>
       <c r="P18" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="Q18" s="10" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="R18" s="10" t="s">
         <v>82</v>
@@ -2095,25 +2098,25 @@
         <v>66</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>71</v>
@@ -2125,22 +2128,22 @@
         <v>32</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="N19" s="7" t="s">
         <v>60</v>
       </c>
       <c r="O19" s="5" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="P19" s="7" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="Q19" s="7" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="R19" s="7" t="s">
         <v>82</v>
@@ -2163,28 +2166,28 @@
     </row>
     <row r="20" spans="1:23" ht="30" customHeight="1">
       <c r="A20" s="8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>26</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="I20" s="8" t="s">
         <v>31</v>
@@ -2196,10 +2199,10 @@
         <v>32</v>
       </c>
       <c r="L20" s="10" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="M20" s="9" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="N20" s="10" t="s">
         <v>60</v>
@@ -2211,7 +2214,7 @@
         <v>69</v>
       </c>
       <c r="Q20" s="10" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="R20" s="10" t="s">
         <v>54</v>
@@ -2234,28 +2237,28 @@
     </row>
     <row r="21" spans="1:23" ht="45" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E21" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="F21" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="F21" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G21" s="7" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>23</v>
@@ -2267,25 +2270,25 @@
         <v>32</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="N21" s="7" t="s">
         <v>50</v>
       </c>
       <c r="O21" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="P21" s="7" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="Q21" s="7" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="R21" s="7" t="s">
-        <v>150</v>
+        <v>94</v>
       </c>
       <c r="S21" s="7" t="s">
         <v>40</v>
@@ -2297,36 +2300,36 @@
         <v>42</v>
       </c>
       <c r="V21" s="7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="W21" s="7" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:23" ht="30" customHeight="1">
       <c r="A22" s="8" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>78</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I22" s="8" t="s">
         <v>55</v>
@@ -2338,22 +2341,22 @@
         <v>32</v>
       </c>
       <c r="L22" s="10" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M22" s="9" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="N22" s="10" t="s">
         <v>50</v>
       </c>
       <c r="O22" s="8" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="P22" s="10" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="Q22" s="10" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="R22" s="10" t="s">
         <v>39</v>
@@ -2368,36 +2371,36 @@
         <v>42</v>
       </c>
       <c r="V22" s="10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="W22" s="10" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:23" ht="30" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>78</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>23</v>
@@ -2409,25 +2412,25 @@
         <v>32</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="N23" s="7" t="s">
         <v>60</v>
       </c>
       <c r="O23" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="P23" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="Q23" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="R23" s="7" t="s">
-        <v>150</v>
+        <v>94</v>
       </c>
       <c r="S23" s="7" t="s">
         <v>40</v>
@@ -2439,33 +2442,33 @@
         <v>42</v>
       </c>
       <c r="V23" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="W23" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:23" ht="30" customHeight="1">
       <c r="A24" s="8" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>78</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H24" s="10" t="s">
         <v>91</v>
@@ -2480,22 +2483,22 @@
         <v>32</v>
       </c>
       <c r="L24" s="10" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="M24" s="9" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="N24" s="10" t="s">
         <v>35</v>
       </c>
       <c r="O24" s="8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="P24" s="10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Q24" s="10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="R24" s="10" t="s">
         <v>54</v>
@@ -2510,33 +2513,33 @@
         <v>42</v>
       </c>
       <c r="V24" s="10" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="W24" s="10" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="25" spans="1:23" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>78</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>91</v>
@@ -2551,22 +2554,22 @@
         <v>32</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="M25" s="6" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="N25" s="7" t="s">
         <v>35</v>
       </c>
       <c r="O25" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="P25" s="7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="Q25" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="R25" s="7" t="s">
         <v>54</v>
@@ -2581,33 +2584,33 @@
         <v>42</v>
       </c>
       <c r="V25" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="W25" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:23" ht="30" customHeight="1">
       <c r="A26" s="8" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>78</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H26" s="10" t="s">
         <v>91</v>
@@ -2622,22 +2625,22 @@
         <v>32</v>
       </c>
       <c r="L26" s="10" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="M26" s="9" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="N26" s="10" t="s">
         <v>35</v>
       </c>
       <c r="O26" s="8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="P26" s="10" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="Q26" s="10" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="R26" s="10" t="s">
         <v>54</v>
@@ -2652,10 +2655,10 @@
         <v>42</v>
       </c>
       <c r="V26" s="10" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="W26" s="10" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -2681,22 +2684,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="11" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-soundcard@e9993308803a85a712f85b8a2b63a62976777825 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Positional/pedalboard-soundcard-bom.xlsx
+++ b/latest/BoM/Positional/pedalboard-soundcard-bom.xlsx
@@ -2388,7 +2388,7 @@
         <v>165</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>156</v>
+        <v>91</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>166</v>
@@ -2459,7 +2459,7 @@
         <v>177</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>156</v>
+        <v>91</v>
       </c>
       <c r="E24" s="10" t="s">
         <v>178</v>
@@ -2530,7 +2530,7 @@
         <v>187</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>156</v>
+        <v>91</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>188</v>
@@ -2601,7 +2601,7 @@
         <v>187</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>156</v>
+        <v>91</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>198</v>

</xml_diff>